<commit_message>
delete operation code in this file
</commit_message>
<xml_diff>
--- a/command-coding.xlsx
+++ b/command-coding.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
   <si>
     <t>指令</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -73,48 +73,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>00000001</t>
-  </si>
-  <si>
-    <t>00000003</t>
-  </si>
-  <si>
-    <t>00000004</t>
-  </si>
-  <si>
-    <t>00000005</t>
-  </si>
-  <si>
-    <t>00000006</t>
-  </si>
-  <si>
-    <t>00000007</t>
-  </si>
-  <si>
-    <t>00000008</t>
-  </si>
-  <si>
-    <t>00000009</t>
-  </si>
-  <si>
-    <t>00000010</t>
-  </si>
-  <si>
-    <t>00000011</t>
-  </si>
-  <si>
-    <t>00000012</t>
-  </si>
-  <si>
-    <t>00000013</t>
-  </si>
-  <si>
-    <t>00000014</t>
-  </si>
-  <si>
-    <t>00000015</t>
-  </si>
-  <si>
     <t>DR←DR+SR</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -194,15 +152,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>00000017</t>
-  </si>
-  <si>
-    <t>00000018</t>
-  </si>
-  <si>
-    <t>00000019</t>
-  </si>
-  <si>
     <t>****</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -211,9 +160,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>00000020</t>
-  </si>
-  <si>
     <t>跳转指令</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -275,18 +221,6 @@
   </si>
   <si>
     <t>SR 出栈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00000000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00000002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>操作码</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -330,9 +264,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -623,415 +556,350 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.875" customWidth="1"/>
-    <col min="3" max="3" width="15.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="6" max="6" width="19.75" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="5" max="5" width="19.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>71</v>
+      <c r="C2" t="s">
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3">
+      <c r="C3">
         <v>2</v>
       </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
       <c r="E3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
+      <c r="C4">
         <v>2</v>
       </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
       <c r="E4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
       <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
       <c r="E5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6">
+      <c r="C6">
         <v>2</v>
       </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
       <c r="E6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7">
+      <c r="C7">
         <v>2</v>
       </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
       <c r="E7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
       <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8">
+        <v>23</v>
+      </c>
+      <c r="C8">
         <v>2</v>
       </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
       <c r="E8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9">
+      <c r="C9">
         <v>2</v>
       </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
       <c r="E9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
       <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
       <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
       <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
-      </c>
-      <c r="F12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>68</v>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:C1"/>
     <mergeCell ref="A3:A13"/>
     <mergeCell ref="A14:A18"/>
     <mergeCell ref="A19:A22"/>

</xml_diff>